<commit_message>
POM Updated script ( Create,delete ==> Cust. & project)
</commit_message>
<xml_diff>
--- a/com.AutomationFramework/src/test/resources/testData.xlsx
+++ b/com.AutomationFramework/src/test/resources/testData.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\karis\git\SeleniumE1\com.AutomationFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34A02B39-1FB3-4754-BC12-7DD6D2AC7F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE14847B-1DB5-4145-8EF2-EAB05CB79953}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="invalidcreds" sheetId="1" r:id="rId1"/>
     <sheet name="managercreds" sheetId="2" r:id="rId2"/>
+    <sheet name="taskspagedetails" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>username</t>
   </si>
@@ -77,6 +78,18 @@
   </si>
   <si>
     <t>Kohli</t>
+  </si>
+  <si>
+    <t>cutomerName</t>
+  </si>
+  <si>
+    <t>projectName</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>WebApplication</t>
   </si>
 </sst>
 </file>
@@ -106,7 +119,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -234,11 +247,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,12 +290,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -618,7 +647,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5EA758-2EF8-4D19-A88B-BC52EB12524C}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -630,16 +659,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="13" t="s">
         <v>13</v>
       </c>
     </row>
@@ -650,11 +679,46 @@
       <c r="B2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF25A03D-D5B6-4D8E-A222-616CE4B62B8B}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" customWidth="1"/>
+    <col min="2" max="2" width="15.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>